<commit_message>
Updated my files and the documentation checklist
</commit_message>
<xml_diff>
--- a/Docs/Documentation Checklist.xlsx
+++ b/Docs/Documentation Checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Source File</t>
   </si>
@@ -339,16 +339,16 @@
   </sheetPr>
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A11" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B33" activeCellId="0" pane="topLeft" sqref="B33"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A51" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B70" activeCellId="0" pane="topLeft" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.4705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.7019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.8313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.93725490196078"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="20.75" outlineLevel="0" r="1" s="1">
@@ -380,7 +380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>7</v>
       </c>
@@ -427,13 +427,16 @@
       <c r="A15" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>18</v>
       </c>
@@ -506,7 +509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>32</v>
       </c>
@@ -533,6 +536,9 @@
       <c r="A38" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
@@ -659,14 +665,20 @@
         <v>59</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="70">
+      <c r="B69" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
         <v>61</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.75" outlineLevel="0" r="72">

</xml_diff>